<commit_message>
Small edit done for NodeURL input
Signed-off-by: paviyaa <senthilkumarjs67@gmail.com>
</commit_message>
<xml_diff>
--- a/test-output/Output Files/ExecutionReport.xlsx
+++ b/test-output/Output Files/ExecutionReport.xlsx
@@ -12,30 +12,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>SearchByBrand Test: STARTED</t>
+    <t>Usedcarschn Test: STARTED</t>
   </si>
   <si>
-    <t>SearchByBrand Test Case: startBrowser Test Method: SUCCESS</t>
+    <t>Usedcarschn Test Case: startBrowser Test Method: SUCCESS</t>
   </si>
   <si>
-    <t>SearchByBrand Test Case: clickSearchBikesFromDrpdwn Test Method: SUCCESS</t>
+    <t>Usedcarschn Test Case: clickSearchUsedCarsFromDrpdwn Test Method: SUCCESS</t>
   </si>
   <si>
-    <t>SearchByBrand Test Case: navigateToNewBikesPage Test Method: SUCCESS</t>
+    <t>Usedcarschn Test Case: navigateToUsedCarsPage Test Method: SUCCESS</t>
   </si>
   <si>
-    <t>SearchByBrand Test Case: navigateToNewBikesSearchPage Test Method: SUCCESS</t>
+    <t>Usedcarschn Test Case: outputDisplay Test Method: SUCCESS</t>
   </si>
   <si>
-    <t>SearchByBrand Test Case: setBrandFilter Test Method: SUCCESS</t>
-  </si>
-  <si>
-    <t>SearchByBrand Test Case: outputDisplay Test Method: SUCCESS</t>
-  </si>
-  <si>
-    <t>SearchByBrand Test: ENDED</t>
+    <t>Usedcarschn Test: ENDED</t>
   </si>
 </sst>
 </file>
@@ -80,7 +74,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -116,16 +110,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Editted for Website Update
Signed-off-by: paviyaa <senthilkumarjs67@gmail.com>
</commit_message>
<xml_diff>
--- a/test-output/Output Files/ExecutionReport.xlsx
+++ b/test-output/Output Files/ExecutionReport.xlsx
@@ -14,22 +14,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>Usedcarschn Test: STARTED</t>
+    <t>UpcomingRequirement Test: STARTED</t>
   </si>
   <si>
-    <t>Usedcarschn Test Case: startBrowser Test Method: SUCCESS</t>
+    <t>UpcomingRequirement Test Case: startBrowser Test Method: SUCCESS</t>
   </si>
   <si>
-    <t>Usedcarschn Test Case: clickSearchUsedCarsFromDrpdwn Test Method: SUCCESS</t>
+    <t>UpcomingRequirement Test Case: loadUpcomingBikesPage Test Method: SUCCESS</t>
   </si>
   <si>
-    <t>Usedcarschn Test Case: navigateToUsedCarsPage Test Method: SUCCESS</t>
+    <t>UpcomingRequirement Test Case: navigateToUpcomingBikesPage Test Method: SUCCESS</t>
   </si>
   <si>
-    <t>Usedcarschn Test Case: outputDisplay Test Method: SUCCESS</t>
+    <t>UpcomingRequirement Test Case: outputDisplay Test Method: SUCCESS</t>
   </si>
   <si>
-    <t>Usedcarschn Test: ENDED</t>
+    <t>UpcomingRequirement Test: ENDED</t>
   </si>
 </sst>
 </file>

</xml_diff>